<commit_message>
aggiornamento librerie alex e test AQR
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/test/Unit Test_Rapporto avanzamento test_AQR.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/test/Unit Test_Rapporto avanzamento test_AQR.xlsx
@@ -21,8 +21,8 @@
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId4"/>
-    <pivotCache cacheId="8" r:id="rId5"/>
+    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="17" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -163,20 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eventuali informazioni relative a dati di input e precondizioni necessarie per l'esecuzione del test, dettagli sugli esiti e varie</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="1" shapeId="0">
+    <comment ref="J3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -191,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J3" authorId="0" shapeId="0">
+    <comment ref="K3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -205,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="1" shapeId="0">
+    <comment ref="L3" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L3" authorId="0" shapeId="0">
+    <comment ref="M3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -240,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="89">
   <si>
     <t>Applicazione</t>
   </si>
@@ -339,9 +326,6 @@
   </si>
   <si>
     <t>MdC_PRJXXXXXX_Step_001</t>
-  </si>
-  <si>
-    <t>Note fornitore</t>
   </si>
   <si>
     <t>Data consegna</t>
@@ -511,14 +495,80 @@
     <t>ind_221 = 1</t>
   </si>
   <si>
-    <t>SNDG:
-0000000090890463
-0000000078356193
-0000000078424764
-0000000078276761
-0000000091605514
-0000000078375153
-0000000078400570</t>
+    <t>SNDG - segment CORPORATE</t>
+  </si>
+  <si>
+    <t>SNDG - segment RETAIL</t>
+  </si>
+  <si>
+    <t>78276761
+90890463
+91605514
+78375153
+78356193</t>
+  </si>
+  <si>
+    <t>86511100
+78297134</t>
+  </si>
+  <si>
+    <t>78276761
+90890463
+91605514
+78375153
+78424764
+83713674</t>
+  </si>
+  <si>
+    <t>78276761
+78400570
+90890463
+91605514
+78375153
+78424764</t>
+  </si>
+  <si>
+    <t>78234149
+78301578</t>
+  </si>
+  <si>
+    <t>78400570
+90890463
+91605514
+78375153
+78356193
+78424764
+78426070</t>
+  </si>
+  <si>
+    <t>78276761
+78400570
+91605514
+78375153
+78424764</t>
+  </si>
+  <si>
+    <t>87986803
+78300922
+78356868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+87986803
+86511100
+78300922
+78297134
+78356868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+90890463
+78356193
+78424764
+78276761
+91605514
+78375153
+78400570</t>
   </si>
 </sst>
 </file>
@@ -1127,7 +1177,7 @@
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1298,9 +1348,6 @@
     <xf numFmtId="0" fontId="16" fillId="6" borderId="14" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1312,52 +1359,52 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1379,15 +1426,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1431,6 +1469,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1441,6 +1503,499 @@
   </cellStyles>
   <dxfs count="203">
     <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <top/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <top/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <bgColor theme="4" tint="0.79998168889431442"/>
@@ -1794,10 +2349,74 @@
       </border>
     </dxf>
     <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -1816,64 +2435,212 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color theme="4" tint="0.79998168889431442"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <top/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <top/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <bottom/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color theme="3"/>
+        </left>
+        <right style="medium">
+          <color theme="3"/>
+        </right>
+        <top style="medium">
+          <color theme="3"/>
+        </top>
+        <bottom style="medium">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="3"/>
+        </left>
+        <right style="thin">
+          <color theme="3"/>
+        </right>
+        <top style="thin">
+          <color theme="3"/>
+        </top>
+        <bottom style="thin">
+          <color theme="3"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -1988,116 +2755,64 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <top/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <top/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="0.79998168889431442"/>
+      </font>
     </dxf>
     <dxf>
       <border>
@@ -2116,170 +2831,10 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
+      <alignment horizontal="center" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" readingOrder="0"/>
     </dxf>
     <dxf>
       <border>
@@ -2633,499 +3188,6 @@
           <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="3"/>
-        </left>
-        <right style="thin">
-          <color theme="3"/>
-        </right>
-        <top style="thin">
-          <color theme="3"/>
-        </top>
-        <bottom style="thin">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <bottom/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <top/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <top/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="0.79998168889431442"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color theme="3"/>
-        </left>
-        <right style="medium">
-          <color theme="3"/>
-        </right>
-        <top style="medium">
-          <color theme="3"/>
-        </top>
-        <bottom style="medium">
-          <color theme="3"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3189,63 +3251,9 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Dessi, Michele" refreshedDate="42744.660268402775" createdVersion="4" refreshedVersion="5" minRefreshableVersion="3" recordCount="14">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Dessi, Michele" refreshedDate="42747.669578240741" createdVersion="4" refreshedVersion="5" minRefreshableVersion="3" recordCount="21">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A3:K1048576" sheet="Lista dei casi di test"/>
-  </cacheSource>
-  <cacheFields count="11">
-    <cacheField name="Applicazione" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="ID" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="8"/>
-    </cacheField>
-    <cacheField name="Funzioni oggetto del test" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Moduli oggetto del test" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Nome del test" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Descrizione test" numFmtId="0">
-      <sharedItems containsBlank="1" longText="1"/>
-    </cacheField>
-    <cacheField name="Esito atteso" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Note fornitore" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-    <cacheField name="Stato test" numFmtId="0">
-      <sharedItems containsBlank="1" count="5">
-        <s v="Ok"/>
-        <m/>
-        <s v="Da eseguire" u="1"/>
-        <s v="Ko" u="1"/>
-        <s v="In esecuzione" u="1"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="Data consegna" numFmtId="14">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-10-28T00:00:00" maxDate="2016-12-23T00:00:00"/>
-    </cacheField>
-    <cacheField name="Verifica DSI" numFmtId="0">
-      <sharedItems containsBlank="1"/>
-    </cacheField>
-  </cacheFields>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Dessi, Michele" refreshedDate="42744.660271527777" createdVersion="4" refreshedVersion="5" minRefreshableVersion="3" recordCount="21">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="A3:L1048576" sheet="Lista dei casi di test"/>
+    <worksheetSource ref="A3:M1048576" sheet="Lista dei casi di test"/>
   </cacheSource>
   <cacheFields count="12">
     <cacheField name="Applicazione" numFmtId="0">
@@ -3303,194 +3311,61 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="14">
-  <r>
-    <m/>
-    <n v="1"/>
-    <m/>
-    <m/>
-    <s v="Indicator 221 - Past due public creditors / employees"/>
-    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• Il flag è valorizzato a 1 se si verifica la presenza di un past due verso impiegati e creditori pubblici;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• La materialità dell’importo è expert-based, per cui è affidato interamente al giudizio del gestore  (CRMD non definisce al momento alcuna linea guida);_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
-    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-12-22T00:00:00"/>
-    <s v="Non verificato"/>
-  </r>
-  <r>
-    <m/>
-    <n v="2"/>
-    <m/>
-    <m/>
-    <s v="Indicator 222 - Collateral Value Decrease"/>
-    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• Il flag è valorizzato a 1 se si verifica la presenza di una significativa riduzione del valore del collateral qualora la vendita dello stesso sia necessaria per il rimborso del finanziamento;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• La materialità dell’importo / percentuale della riduzione è expert-based, per cui è affidato interamente al giudizio del gestore (CRMD non definisce al momento alcuna linea guida);_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
-    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-12-22T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <n v="3"/>
-    <m/>
-    <m/>
-    <s v="Indicator 223 - Delta Cashflow"/>
-    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• L’indicatore è valorizzato a 1 se si verifica un decremento significativo nei flussi di cassa futuri previsionali;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• La materialità dell’importo / percentuale della riduzione è expert-based, per cui è affidato interamente al giudizio del gestore (CRMD non definisce al momento alcuna linea guida);_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
-    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-12-22T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <n v="4"/>
-    <m/>
-    <m/>
-    <s v="Indicator 224 - Covenant Breach"/>
-    <s v="• Per il singolo SNDG l’indicatore ha il seguente dominio (seguirà traduzione): _x000a_o COVENANT ROTTO NON ANCORA SANATO_x000a_o COVENANT IN TENSIONE_x000a_o COVENANT SCADUTO E NON MONITORATO _x000a_o COVENANT NON RISPETTATO E NON SANATO _x000a__x000a_• Lasciamo all’IT la scelta tra le seguenti modalità di inserimento a cruscotto e nel repository dei dati delle informazioni relative a questo trigger_x000a_o MODALITA’ 1_x000a_A cruscotto viene evidenziata una domanda a risposta multipla sui covenant;_x000a_Nel datamart EWS verrà storicizzata un’unica variabile valorizzata con un codice (ad. es. 01 = covenant rotto non ancora sanato, 02 = etc….);_x000a__x000a_o MODALITA’ 2_x000a_A cruscotto vengono evidenziate 4 domande afferenti i covenant; _x000a_Nel datamart EWS verranno storicizzate 4 variabili flag, il cui valore può essere pari a 0 o 1, corrispondenti a ciascuna domanda del cruscotto._x000a__x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• L’indicatore è attualmente manuale e non sono possibili casi di errore, ma nelle successive versioni dovranno essere previsti dei controlli._x000a_"/>
-    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-12-22T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <n v="5"/>
-    <m/>
-    <m/>
-    <s v="Indicator 225 - Bond Trade Suspended"/>
-    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• L’indicatore è valorizzato a 1 se si verifica una sospensione temporanea alla negoziazione di un bond per momentanea difficoltà della controparte emittente;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
-    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-12-22T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <n v="6"/>
-    <m/>
-    <m/>
-    <s v="BR15"/>
-    <s v="ind_221 = 1"/>
-    <s v="accensione della BR 15"/>
-    <s v="SNDG:_x000a_0000000090890463_x000a_0000000078356193_x000a_0000000078424764_x000a_0000000078276761_x000a_0000000091605514_x000a_0000000078375153_x000a_0000000078400570"/>
-    <x v="0"/>
-    <d v="2016-10-28T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <n v="7"/>
-    <m/>
-    <m/>
-    <s v="BR16"/>
-    <s v="ind_225 = 1"/>
-    <s v="accensione della BR 16"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-10-28T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <n v="8"/>
-    <m/>
-    <m/>
-    <s v="ECCEZIONE_1"/>
-    <s v="BR15 = 1 or BR16 = 1"/>
-    <s v="accensione ECCEZIONE_1 e assegnamento colore LIGHT_BLUE"/>
-    <m/>
-    <x v="0"/>
-    <d v="2016-10-28T00:00:00"/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="1"/>
-    <m/>
-    <m/>
-  </r>
-</pivotCacheRecords>
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Dessi, Michele" refreshedDate="42747.669579861111" createdVersion="4" refreshedVersion="5" minRefreshableVersion="3" recordCount="14">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A3:L1048576" sheet="Lista dei casi di test"/>
+  </cacheSource>
+  <cacheFields count="11">
+    <cacheField name="Applicazione" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="ID" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="8"/>
+    </cacheField>
+    <cacheField name="Funzioni oggetto del test" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Moduli oggetto del test" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Nome del test" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Descrizione test" numFmtId="0">
+      <sharedItems containsBlank="1" longText="1"/>
+    </cacheField>
+    <cacheField name="Esito atteso" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Note fornitore" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Stato test" numFmtId="0">
+      <sharedItems containsBlank="1" count="5">
+        <s v="Ok"/>
+        <m/>
+        <s v="Da eseguire" u="1"/>
+        <s v="Ko" u="1"/>
+        <s v="In esecuzione" u="1"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Data consegna" numFmtId="14">
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2016-10-28T00:00:00" maxDate="2016-12-23T00:00:00"/>
+    </cacheField>
+    <cacheField name="Verifica DSI" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="21">
   <r>
     <m/>
@@ -3789,8 +3664,407 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="14">
+  <r>
+    <m/>
+    <n v="1"/>
+    <m/>
+    <m/>
+    <s v="Indicator 221 - Past due public creditors / employees"/>
+    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• Il flag è valorizzato a 1 se si verifica la presenza di un past due verso impiegati e creditori pubblici;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• La materialità dell’importo è expert-based, per cui è affidato interamente al giudizio del gestore  (CRMD non definisce al momento alcuna linea guida);_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
+    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-12-22T00:00:00"/>
+    <s v="Non verificato"/>
+  </r>
+  <r>
+    <m/>
+    <n v="2"/>
+    <m/>
+    <m/>
+    <s v="Indicator 222 - Collateral Value Decrease"/>
+    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• Il flag è valorizzato a 1 se si verifica la presenza di una significativa riduzione del valore del collateral qualora la vendita dello stesso sia necessaria per il rimborso del finanziamento;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• La materialità dell’importo / percentuale della riduzione è expert-based, per cui è affidato interamente al giudizio del gestore (CRMD non definisce al momento alcuna linea guida);_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
+    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-12-22T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <n v="3"/>
+    <m/>
+    <m/>
+    <s v="Indicator 223 - Delta Cashflow"/>
+    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• L’indicatore è valorizzato a 1 se si verifica un decremento significativo nei flussi di cassa futuri previsionali;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• La materialità dell’importo / percentuale della riduzione è expert-based, per cui è affidato interamente al giudizio del gestore (CRMD non definisce al momento alcuna linea guida);_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
+    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-12-22T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <n v="4"/>
+    <m/>
+    <m/>
+    <s v="Indicator 224 - Covenant Breach"/>
+    <s v="• Per il singolo SNDG l’indicatore ha il seguente dominio (seguirà traduzione): _x000a_o COVENANT ROTTO NON ANCORA SANATO_x000a_o COVENANT IN TENSIONE_x000a_o COVENANT SCADUTO E NON MONITORATO _x000a_o COVENANT NON RISPETTATO E NON SANATO _x000a__x000a_• Lasciamo all’IT la scelta tra le seguenti modalità di inserimento a cruscotto e nel repository dei dati delle informazioni relative a questo trigger_x000a_o MODALITA’ 1_x000a_A cruscotto viene evidenziata una domanda a risposta multipla sui covenant;_x000a_Nel datamart EWS verrà storicizzata un’unica variabile valorizzata con un codice (ad. es. 01 = covenant rotto non ancora sanato, 02 = etc….);_x000a__x000a_o MODALITA’ 2_x000a_A cruscotto vengono evidenziate 4 domande afferenti i covenant; _x000a_Nel datamart EWS verranno storicizzate 4 variabili flag, il cui valore può essere pari a 0 o 1, corrispondenti a ciascuna domanda del cruscotto._x000a__x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• L’indicatore è attualmente manuale e non sono possibili casi di errore, ma nelle successive versioni dovranno essere previsti dei controlli._x000a_"/>
+    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-12-22T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <n v="5"/>
+    <m/>
+    <m/>
+    <s v="Indicator 225 - Bond Trade Suspended"/>
+    <s v="• Per il singolo SNDG il campo può assumere valore 0 o 1 a seconda che venga attivato o meno il flag sul cruscotto;_x000a_• L’indicatore è valorizzato a 1 se si verifica una sospensione temporanea alla negoziazione di un bond per momentanea difficoltà della controparte emittente;_x000a_• L’alimentazione è manuale attraverso l’applicativo “cruscotto” a cura del gestore della posizione;_x000a_• L’indicatore è manuale e non sono previsti possibili casi di errore._x000a_"/>
+    <s v=" - porting variabile_x000a__x000a_ - ERRORE - considerat i seguendi casi:_x000a_indicatore è missing -&gt; missing"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-12-22T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <n v="6"/>
+    <m/>
+    <m/>
+    <s v="BR15"/>
+    <s v="ind_221 = 1"/>
+    <s v="accensione della BR 15"/>
+    <s v="SNDG:_x000a_0000000090890463_x000a_0000000078356193_x000a_0000000078424764_x000a_0000000078276761_x000a_0000000091605514_x000a_0000000078375153_x000a_0000000078400570"/>
+    <x v="0"/>
+    <d v="2016-10-28T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <n v="7"/>
+    <m/>
+    <m/>
+    <s v="BR16"/>
+    <s v="ind_225 = 1"/>
+    <s v="accensione della BR 16"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-10-28T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <n v="8"/>
+    <m/>
+    <m/>
+    <s v="ECCEZIONE_1"/>
+    <s v="BR15 = 1 or BR16 = 1"/>
+    <s v="accensione ECCEZIONE_1 e assegnamento colore LIGHT_BLUE"/>
+    <m/>
+    <x v="0"/>
+    <d v="2016-10-28T00:00:00"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella pivot3" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Stato Casi Test">
+  <location ref="B7:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="11">
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow">
+      <items count="6">
+        <item h="1" m="1" x="2"/>
+        <item h="1" m="1" x="4"/>
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Conteggio" fld="1" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="44">
+    <format dxfId="145">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="144">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="143">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="142">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="141">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="140">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="139">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="138">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="137">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="136">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="135">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="134">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="133">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="132">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="131">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="130">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="129">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="128">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="127">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="126">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="125">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="124">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="123">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="122">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="121">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="120">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="119">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="118">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="117">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="116">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="115">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="114">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="113">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="112">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="111">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="110">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="109">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="108">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="107">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="106">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="105">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="104">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="8" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="103">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="102">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella pivot3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H10:I14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -3838,107 +4112,107 @@
     <dataField name="Conteggio" fld="1" subtotal="count" baseField="10" baseItem="0"/>
   </dataFields>
   <formats count="29">
-    <format dxfId="129">
+    <format dxfId="174">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="128">
+    <format dxfId="173">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="127">
+    <format dxfId="172">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="126">
+    <format dxfId="171">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="125">
+    <format dxfId="170">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="124">
+    <format dxfId="169">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="10" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="123">
+    <format dxfId="168">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="122">
+    <format dxfId="167">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="121">
+    <format dxfId="166">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="120">
+    <format dxfId="165">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="119">
+    <format dxfId="164">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="118">
+    <format dxfId="163">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="117">
+    <format dxfId="162">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="10" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="116">
+    <format dxfId="161">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="115">
+    <format dxfId="160">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="114">
+    <format dxfId="159">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="113">
+    <format dxfId="158">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="112">
+    <format dxfId="157">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="111">
+    <format dxfId="156">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="110">
+    <format dxfId="155">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="10" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="109">
+    <format dxfId="154">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="108">
+    <format dxfId="153">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="107">
+    <format dxfId="152">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="106">
+    <format dxfId="151">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="105">
+    <format dxfId="150">
       <pivotArea field="10" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="104">
+    <format dxfId="149">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="103">
+    <format dxfId="148">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="10" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="102">
+    <format dxfId="147">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="101">
+    <format dxfId="146">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -3951,8 +4225,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella pivot2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella pivot2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L10:M13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -3997,308 +4271,96 @@
     <dataField name="Conteggio" fld="1" subtotal="count" baseField="11" baseItem="0"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="157">
+    <format dxfId="202">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="156">
+    <format dxfId="201">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="155">
+    <format dxfId="200">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="154">
+    <format dxfId="199">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="153">
+    <format dxfId="198">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="152">
+    <format dxfId="197">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="151">
+    <format dxfId="196">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="150">
+    <format dxfId="195">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="11" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="149">
+    <format dxfId="194">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="148">
+    <format dxfId="193">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="147">
+    <format dxfId="192">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="146">
+    <format dxfId="191">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="145">
+    <format dxfId="190">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="144">
+    <format dxfId="189">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="143">
+    <format dxfId="188">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="142">
+    <format dxfId="187">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="141">
+    <format dxfId="186">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="140">
+    <format dxfId="185">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="139">
+    <format dxfId="184">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="138">
+    <format dxfId="183">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="137">
+    <format dxfId="182">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="136">
+    <format dxfId="181">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="135">
+    <format dxfId="180">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="134">
+    <format dxfId="179">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="11" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="133">
+    <format dxfId="178">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="132">
+    <format dxfId="177">
       <pivotArea field="11" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="131">
+    <format dxfId="176">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="130">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Stato Casi Test">
-  <location ref="B7:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="11">
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow">
-      <items count="6">
-        <item h="1" m="1" x="2"/>
-        <item h="1" m="1" x="4"/>
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="8"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Conteggio" fld="1" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <formats count="44">
-    <format dxfId="201">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="200">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="199">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="198">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="197">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="196">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="195">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="194">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="193">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="192">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="191">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="190">
-      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="189">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="188">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="187">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="186">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="185">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="184">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="183">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="182">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="181">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="180">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="179">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="178">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="177">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="176">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
     <format dxfId="175">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="174">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="173">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="172">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="171">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="170">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="169">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="168">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="167">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="166">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="165">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="164">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="163">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="162">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="161">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="160">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="8" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="159">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="158">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -4958,80 +5020,80 @@
     </row>
     <row r="24" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="79"/>
+      <c r="B24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="83"/>
+      <c r="K24" s="84"/>
       <c r="L24" s="7"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="80" t="s">
+      <c r="B25" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="81"/>
-      <c r="D25" s="81"/>
-      <c r="E25" s="81"/>
-      <c r="F25" s="81"/>
-      <c r="G25" s="81"/>
-      <c r="H25" s="81"/>
-      <c r="I25" s="81"/>
-      <c r="J25" s="81"/>
-      <c r="K25" s="82"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
+      <c r="K25" s="87"/>
       <c r="L25" s="7"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="81"/>
-      <c r="I26" s="81"/>
-      <c r="J26" s="81"/>
-      <c r="K26" s="82"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
+      <c r="K26" s="87"/>
       <c r="L26" s="7"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
-      <c r="B27" s="80" t="s">
+      <c r="B27" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
-      <c r="F27" s="81"/>
-      <c r="G27" s="81"/>
-      <c r="H27" s="81"/>
-      <c r="I27" s="81"/>
-      <c r="J27" s="81"/>
-      <c r="K27" s="82"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
+      <c r="K27" s="87"/>
       <c r="L27" s="7"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
-      <c r="B28" s="83"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
-      <c r="K28" s="85"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="89"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="89"/>
+      <c r="G28" s="89"/>
+      <c r="H28" s="89"/>
+      <c r="I28" s="89"/>
+      <c r="J28" s="89"/>
+      <c r="K28" s="90"/>
       <c r="L28" s="7"/>
       <c r="M28" s="1"/>
     </row>
@@ -5157,161 +5219,161 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="76" t="s">
+      <c r="C37" s="76"/>
+      <c r="D37" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="76"/>
-      <c r="F37" s="76"/>
-      <c r="G37" s="76"/>
-      <c r="H37" s="76"/>
-      <c r="I37" s="76"/>
-      <c r="J37" s="76"/>
-      <c r="K37" s="76"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="77"/>
+      <c r="J37" s="77"/>
+      <c r="K37" s="77"/>
       <c r="L37" s="7"/>
       <c r="M37" s="1"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="76" t="s">
+      <c r="C38" s="76"/>
+      <c r="D38" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="E38" s="76"/>
-      <c r="F38" s="76"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="76"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="77"/>
+      <c r="I38" s="77"/>
+      <c r="J38" s="77"/>
+      <c r="K38" s="77"/>
       <c r="L38" s="7"/>
       <c r="M38" s="1"/>
     </row>
     <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C39" s="75"/>
-      <c r="D39" s="76" t="s">
+      <c r="C39" s="76"/>
+      <c r="D39" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="E39" s="76"/>
-      <c r="F39" s="76"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
-      <c r="K39" s="76"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="77"/>
+      <c r="J39" s="77"/>
+      <c r="K39" s="77"/>
       <c r="L39" s="7"/>
       <c r="M39" s="1"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="75"/>
-      <c r="D40" s="76" t="s">
+      <c r="C40" s="76"/>
+      <c r="D40" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="76"/>
-      <c r="K40" s="76"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="77"/>
+      <c r="G40" s="77"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="77"/>
+      <c r="J40" s="77"/>
+      <c r="K40" s="77"/>
       <c r="L40" s="7"/>
       <c r="M40" s="1"/>
     </row>
     <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="75"/>
-      <c r="D41" s="76" t="s">
+      <c r="C41" s="76"/>
+      <c r="D41" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="E41" s="76"/>
-      <c r="F41" s="76"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="76"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="77"/>
+      <c r="G41" s="77"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="77"/>
+      <c r="J41" s="77"/>
+      <c r="K41" s="77"/>
       <c r="L41" s="7"/>
       <c r="M41" s="1"/>
     </row>
     <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="75"/>
-      <c r="D42" s="86" t="s">
+      <c r="C42" s="76"/>
+      <c r="D42" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="87"/>
-      <c r="F42" s="76" t="s">
+      <c r="E42" s="80"/>
+      <c r="F42" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76" t="s">
+      <c r="G42" s="77"/>
+      <c r="H42" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="76"/>
+      <c r="I42" s="77"/>
+      <c r="J42" s="77"/>
+      <c r="K42" s="77"/>
       <c r="L42" s="7"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
-      <c r="B43" s="75" t="s">
+      <c r="B43" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="75"/>
-      <c r="D43" s="76" t="s">
+      <c r="C43" s="76"/>
+      <c r="D43" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="E43" s="76"/>
-      <c r="F43" s="76"/>
-      <c r="G43" s="76"/>
-      <c r="H43" s="76"/>
-      <c r="I43" s="76"/>
-      <c r="J43" s="76"/>
-      <c r="K43" s="76"/>
+      <c r="E43" s="77"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="77"/>
+      <c r="H43" s="77"/>
+      <c r="I43" s="77"/>
+      <c r="J43" s="77"/>
+      <c r="K43" s="77"/>
       <c r="L43" s="7"/>
       <c r="M43" s="1"/>
     </row>
     <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="C44" s="75"/>
-      <c r="D44" s="90">
+      <c r="C44" s="76"/>
+      <c r="D44" s="78">
         <v>42506</v>
       </c>
-      <c r="E44" s="91"/>
-      <c r="F44" s="87"/>
-      <c r="G44" s="76" t="s">
+      <c r="E44" s="79"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="H44" s="76"/>
-      <c r="I44" s="76"/>
-      <c r="J44" s="90">
+      <c r="H44" s="77"/>
+      <c r="I44" s="77"/>
+      <c r="J44" s="78">
         <v>42506</v>
       </c>
-      <c r="K44" s="87"/>
+      <c r="K44" s="80"/>
       <c r="L44" s="7"/>
       <c r="M44" s="1"/>
     </row>
@@ -5362,35 +5424,35 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
-      <c r="B48" s="88" t="s">
+      <c r="B48" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="C48" s="88"/>
-      <c r="D48" s="88"/>
-      <c r="E48" s="88"/>
-      <c r="F48" s="88"/>
-      <c r="G48" s="88"/>
-      <c r="H48" s="88"/>
-      <c r="I48" s="88"/>
-      <c r="J48" s="88"/>
-      <c r="K48" s="88"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="74"/>
+      <c r="E48" s="74"/>
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="74"/>
+      <c r="I48" s="74"/>
+      <c r="J48" s="74"/>
+      <c r="K48" s="74"/>
       <c r="L48" s="7"/>
       <c r="M48" s="1"/>
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
-      <c r="B49" s="89" t="s">
+      <c r="B49" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="C49" s="89"/>
-      <c r="D49" s="89"/>
-      <c r="E49" s="89"/>
-      <c r="F49" s="89"/>
-      <c r="G49" s="89"/>
-      <c r="H49" s="89"/>
-      <c r="I49" s="89"/>
-      <c r="J49" s="89"/>
-      <c r="K49" s="89"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
+      <c r="I49" s="75"/>
+      <c r="J49" s="75"/>
+      <c r="K49" s="75"/>
       <c r="L49" s="7"/>
       <c r="M49" s="1"/>
     </row>
@@ -5441,6 +5503,25 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:K37"/>
+    <mergeCell ref="B24:K24"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:K38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="D39:K39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:K40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="D41:K41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:K42"/>
     <mergeCell ref="B48:K48"/>
     <mergeCell ref="B49:K49"/>
     <mergeCell ref="B43:C43"/>
@@ -5449,25 +5530,6 @@
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="G44:I44"/>
     <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:K41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:K42"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="D38:K38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:K39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:K40"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:K37"/>
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="B25:K25"/>
-    <mergeCell ref="B26:K26"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5477,10 +5539,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Foglio2"/>
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="E7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5491,52 +5553,55 @@
     <col min="4" max="4" width="22.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" style="15" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="9.140625" style="15"/>
-    <col min="15" max="17" width="9.140625" style="15" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="15"/>
+    <col min="7" max="7" width="62.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34" style="15" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.140625" style="15"/>
+    <col min="16" max="18" width="9.140625" style="15" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="94" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="93" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="95"/>
-      <c r="G1" s="95"/>
-      <c r="H1" s="95"/>
-      <c r="I1" s="95"/>
-      <c r="J1" s="95"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="97" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="92" t="s">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="96" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" s="91" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="98"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="97"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
@@ -5544,10 +5609,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="14" t="s">
         <v>2</v>
@@ -5559,324 +5624,307 @@
         <v>4</v>
       </c>
       <c r="H3" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>52</v>
-      </c>
       <c r="L3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>37</v>
+        <v>51</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="Q3" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="70"/>
-      <c r="I4" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J4" s="17">
+        <v>63</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="119" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="120" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="17">
         <v>42726</v>
       </c>
-      <c r="K4" s="72" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="73" t="str">
-        <f>IF(K4=I4,"Coerente",(IF(K4="Non verificato","Non applicabile","Non coerente")))</f>
+      <c r="L4" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="72" t="str">
+        <f>IF(L4=J4,"Coerente",(IF(L4="Non verificato","Non applicabile","Non coerente")))</f>
         <v>Non applicabile</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="68" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" s="69" t="s">
-        <v>65</v>
-      </c>
-      <c r="G5" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" s="70"/>
-      <c r="I5" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="17">
+        <v>64</v>
+      </c>
+      <c r="G5" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="119">
+        <v>78247453</v>
+      </c>
+      <c r="I5" s="120" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" s="17">
         <v>42726</v>
       </c>
-      <c r="K5" s="72"/>
-      <c r="L5" s="73"/>
-    </row>
-    <row r="6" spans="1:17" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L5" s="71"/>
+      <c r="M5" s="72"/>
+    </row>
+    <row r="6" spans="1:18" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13">
         <v>3</v>
       </c>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="68" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="G6" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="70"/>
-      <c r="I6" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="17">
+        <v>65</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="119" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="120" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="17">
         <v>42726</v>
       </c>
-      <c r="K6" s="72"/>
-      <c r="L6" s="73"/>
-    </row>
-    <row r="7" spans="1:17" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L6" s="71"/>
+      <c r="M6" s="72"/>
+    </row>
+    <row r="7" spans="1:18" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13"/>
       <c r="B7" s="13">
         <v>4</v>
       </c>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="68" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="69" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" s="70"/>
-      <c r="I7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="17">
+        <v>66</v>
+      </c>
+      <c r="G7" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="119">
+        <v>78425618</v>
+      </c>
+      <c r="I7" s="120" t="s">
+        <v>84</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="17">
         <v>42726</v>
       </c>
-      <c r="K7" s="72"/>
-      <c r="L7" s="73"/>
-    </row>
-    <row r="8" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L7" s="71"/>
+      <c r="M7" s="72"/>
+    </row>
+    <row r="8" spans="1:18" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
       <c r="B8" s="13">
         <v>5</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
       <c r="E8" s="68" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F8" s="69" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="119" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="120" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="17">
+        <v>42726</v>
+      </c>
+      <c r="L8" s="71"/>
+      <c r="M8" s="72"/>
+    </row>
+    <row r="9" spans="1:18" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13">
+        <v>6</v>
+      </c>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" s="70"/>
-      <c r="I8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J8" s="17">
-        <v>42726</v>
-      </c>
-      <c r="K8" s="72"/>
-      <c r="L8" s="73"/>
-    </row>
-    <row r="9" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="73"/>
-    </row>
-    <row r="10" spans="1:17" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="115" t="s">
+        <v>87</v>
+      </c>
+      <c r="I9" s="115" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" s="17">
+        <v>42671</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
       <c r="B10" s="13">
-        <v>6</v>
-      </c>
-      <c r="C10" s="72"/>
-      <c r="D10" s="72"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="74" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="68" t="s">
+      <c r="F10" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="113" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="99" t="s">
-        <v>78</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="17">
+      <c r="H10" s="114"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="17">
         <v>42671</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="1:17" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L10" s="13"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13">
-        <v>7</v>
-      </c>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
+        <v>8</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
       <c r="E11" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="74" t="s">
-        <v>76</v>
+        <v>72</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="100"/>
-      <c r="I11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J11" s="17">
+        <v>74</v>
+      </c>
+      <c r="H11" s="118"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="K11" s="17">
         <v>42671</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13">
-        <v>8</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="H12" s="101"/>
-      <c r="I12" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="17">
-        <v>42671</v>
-      </c>
-      <c r="K12" s="13"/>
-      <c r="L12" s="17"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="17"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="17"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L15" s="18"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L16" s="18"/>
-    </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L17" s="18"/>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L18" s="18"/>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L21" s="18"/>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L22" s="18"/>
-    </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L23" s="18"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M12" s="18"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M13" s="18"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M14" s="18"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M15" s="18"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M16" s="18"/>
+    </row>
+    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M17" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="H10:H12"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="H9:H11"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I1048576">
-      <formula1>$P$3:$P$3</formula1>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J1048576">
+      <formula1>$Q$3:$Q$3</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K1048576">
-      <formula1>$Q$3:$Q$3</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L1048576">
+      <formula1>$R$3:$R$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5916,40 +5964,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="104" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="105"/>
+      <c r="E1" s="106"/>
+      <c r="G1" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="109"/>
-      <c r="C1" s="109"/>
-      <c r="D1" s="109"/>
-      <c r="E1" s="110"/>
-      <c r="G1" s="108" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" s="109"/>
-      <c r="I1" s="109"/>
-      <c r="J1" s="109"/>
-      <c r="K1" s="109"/>
-      <c r="L1" s="109"/>
-      <c r="M1" s="109"/>
-      <c r="N1" s="109"/>
-      <c r="O1" s="110"/>
+      <c r="H1" s="105"/>
+      <c r="I1" s="105"/>
+      <c r="J1" s="105"/>
+      <c r="K1" s="105"/>
+      <c r="L1" s="105"/>
+      <c r="M1" s="105"/>
+      <c r="N1" s="105"/>
+      <c r="O1" s="106"/>
     </row>
     <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="113"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="113"/>
+      <c r="A2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="109"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="109"/>
     </row>
     <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="36"/>
@@ -5975,13 +6023,13 @@
       <c r="E4" s="24"/>
       <c r="G4" s="26"/>
       <c r="H4" s="50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I4" s="51" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" s="52" t="s">
         <v>50</v>
-      </c>
-      <c r="J4" s="52" t="s">
-        <v>51</v>
       </c>
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
@@ -5991,11 +6039,11 @@
     </row>
     <row r="5" spans="1:15" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26"/>
-      <c r="B5" s="102" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="103"/>
-      <c r="D5" s="104"/>
+      <c r="B5" s="98" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" s="100"/>
       <c r="E5" s="24"/>
       <c r="G5" s="26"/>
       <c r="H5" s="53">
@@ -6003,7 +6051,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="54">
-        <f>COUNTIF('Lista dei casi di test'!L:L,"Coerente")+COUNTIF('Lista dei casi di test'!L:L,"Non coerente")</f>
+        <f>COUNTIF('Lista dei casi di test'!M:M,"Coerente")+COUNTIF('Lista dei casi di test'!M:M,"Non coerente")</f>
         <v>0</v>
       </c>
       <c r="J5" s="67">
@@ -6018,9 +6066,9 @@
     </row>
     <row r="6" spans="1:15" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="107"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="103"/>
       <c r="E6" s="24"/>
       <c r="G6" s="26"/>
       <c r="H6" s="48"/>
@@ -6035,13 +6083,13 @@
     <row r="7" spans="1:15" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26"/>
       <c r="B7" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="46" t="s">
-        <v>48</v>
-      </c>
       <c r="D7" s="47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="24"/>
       <c r="G7" s="26"/>
@@ -6057,7 +6105,7 @@
     <row r="8" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="35">
@@ -6066,23 +6114,23 @@
       </c>
       <c r="E8" s="24"/>
       <c r="G8" s="25"/>
-      <c r="H8" s="102" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="103"/>
-      <c r="J8" s="104"/>
+      <c r="H8" s="98" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="99"/>
+      <c r="J8" s="100"/>
       <c r="K8" s="30"/>
-      <c r="L8" s="102" t="s">
-        <v>49</v>
-      </c>
-      <c r="M8" s="103"/>
-      <c r="N8" s="104"/>
+      <c r="L8" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="99"/>
+      <c r="N8" s="100"/>
       <c r="O8" s="24"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39"/>
       <c r="B9" s="57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="44">
         <v>8</v>
@@ -6093,19 +6141,19 @@
       </c>
       <c r="E9" s="24"/>
       <c r="G9" s="39"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="115"/>
-      <c r="J9" s="116"/>
+      <c r="H9" s="110"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="112"/>
       <c r="K9" s="30"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="115"/>
-      <c r="N9" s="116"/>
+      <c r="L9" s="110"/>
+      <c r="M9" s="111"/>
+      <c r="N9" s="112"/>
       <c r="O9" s="24"/>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39"/>
       <c r="B10" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C10" s="45">
         <v>8</v>
@@ -6114,23 +6162,23 @@
       <c r="E10" s="24"/>
       <c r="G10" s="39"/>
       <c r="H10" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" s="65" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J10" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" s="23"/>
       <c r="L10" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M10" s="66" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="N10" s="47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O10" s="24"/>
     </row>
@@ -6142,7 +6190,7 @@
       <c r="E11" s="24"/>
       <c r="G11" s="39"/>
       <c r="H11" s="61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="40">
         <v>1</v>
@@ -6153,7 +6201,7 @@
       </c>
       <c r="K11" s="23"/>
       <c r="L11" s="60" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M11" s="41"/>
       <c r="N11" s="35" t="e">
@@ -6170,7 +6218,7 @@
       <c r="E12" s="24"/>
       <c r="G12" s="39"/>
       <c r="H12" s="60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I12" s="41"/>
       <c r="J12" s="35">
@@ -6179,7 +6227,7 @@
       </c>
       <c r="K12" s="23"/>
       <c r="L12" s="62" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M12" s="41"/>
       <c r="N12" s="35" t="e">
@@ -6196,7 +6244,7 @@
       <c r="E13" s="24"/>
       <c r="G13" s="39"/>
       <c r="H13" s="62" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="41"/>
       <c r="J13" s="35">
@@ -6205,7 +6253,7 @@
       </c>
       <c r="K13" s="23"/>
       <c r="L13" s="62" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M13" s="42"/>
       <c r="N13" s="32"/>
@@ -6219,7 +6267,7 @@
       <c r="E14" s="24"/>
       <c r="G14" s="26"/>
       <c r="H14" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I14" s="42">
         <v>1</v>
@@ -6476,7 +6524,7 @@
     <mergeCell ref="H8:J9"/>
   </mergeCells>
   <conditionalFormatting sqref="J5">
-    <cfRule type="expression" dxfId="202" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>"&lt;25"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6600,18 +6648,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6631,14 +6679,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3A56FCF-C5F4-4BE8-A3D4-155BB73757FB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4C5EE125-43E6-46CF-BE7E-DF899F9AE08F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6651,4 +6691,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3A56FCF-C5F4-4BE8-A3D4-155BB73757FB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>